<commit_message>
Made some changes to the graphs of graduation and next term predictions.
</commit_message>
<xml_diff>
--- a/next_semester_gpa_prediction/TotalResults/next_semest_gpa_prediction_results.xlsx
+++ b/next_semester_gpa_prediction/TotalResults/next_semest_gpa_prediction_results.xlsx
@@ -13,11 +13,12 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>id</t>
   </si>
@@ -114,16 +115,19 @@
     <t>count</t>
   </si>
   <si>
-    <t>normalized GBT</t>
+    <t>term</t>
   </si>
   <si>
-    <t>normalized LR</t>
+    <t>Gradient Boosted Trees</t>
   </si>
   <si>
-    <t>normalized MLPR</t>
+    <t>Linear Regression</t>
   </si>
   <si>
-    <t>normalized ZEROR</t>
+    <t>Neural Network</t>
+  </si>
+  <si>
+    <t>ZeroR</t>
   </si>
 </sst>
 </file>
@@ -181,6 +185,1455 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" b="1" i="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>NRMSE for Next Term GPA Prediction</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$M$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gradient Boosted Trees</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$L$4:$L$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$M$4:$M$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.15360541300650438</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19717511334352919</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17037379566567984</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11401947611795984</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11265050681501694</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.4098153328822655E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.3274726130732761E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1224465756653058</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0335856361957539E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.20128181654328492</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.2578072171061229E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.12728645909545466</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7E16-430B-804B-6FC8E4850680}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$N$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Linear Regression</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$L$4:$L$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$N$4:$N$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.17656964512263512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21581288595893541</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15693791695780912</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11308621993028009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11628547771582466</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.2055575555213419E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.1054044701327336E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.11561297875470511</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.4735674674243334E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.19833259050716653</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.1514943300742719E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.10365831542797982</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7E16-430B-804B-6FC8E4850680}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Neural Network</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$L$4:$L$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$O$4:$O$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.15729495168259933</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.20084127459490678</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17006521969788191</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10608812794165122</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11377927342525836</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.7532515641308429E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.1121891097085509E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.11455833199408673</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.4392586059024596E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.19839802486821512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.5203493904913925E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.5987736950434915E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7E16-430B-804B-6FC8E4850680}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$P$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ZeroR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$L$4:$L$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$P$4:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.24308134186525437</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.37604348961155448</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.31541076825508763</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20817668091810557</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.19140351506661818</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1786756418410746</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.170001548191548</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.20416396800075656</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.3128324848985422E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.13773374538818672</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.7869952397926631E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.16848786946276259</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-7E16-430B-804B-6FC8E4850680}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="504759576"/>
+        <c:axId val="504761544"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="504759576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Term Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="504761544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="504761544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>NRMSE</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="504759576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1076325</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>450274</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>155864</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8672,7 +10125,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -9050,8 +10503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Y47" sqref="Y47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9082,17 +10535,20 @@
       <c r="F3" t="s">
         <v>27</v>
       </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
       <c r="M3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -9131,6 +10587,9 @@
         <f>GETPIVOTDATA("Sum of ZEROR-residual",$A$3,"next term",2)/$F$4</f>
         <v>0.9723253674610175</v>
       </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
       <c r="M4">
         <f>H4/4</f>
         <v>0.15360541300650438</v>
@@ -9184,6 +10643,9 @@
         <f>GETPIVOTDATA("Sum of ZEROR-residual",$A$3,"next term",3)/$F$5</f>
         <v>1.5041739584462179</v>
       </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
       <c r="M5">
         <f t="shared" ref="M5:P16" si="0">H5/4</f>
         <v>0.19717511334352919</v>
@@ -9237,6 +10699,9 @@
         <f>GETPIVOTDATA("Sum of ZEROR-residual",$A$3,"next term",4)/$F$6</f>
         <v>1.2616430730203505</v>
       </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
       <c r="M6">
         <f t="shared" si="0"/>
         <v>0.17037379566567984</v>
@@ -9290,6 +10755,9 @@
         <f>GETPIVOTDATA("Sum of ZEROR-residual",$A$3,"next term",5)/$F$7</f>
         <v>0.83270672367242227</v>
       </c>
+      <c r="L7">
+        <v>5</v>
+      </c>
       <c r="M7">
         <f t="shared" si="0"/>
         <v>0.11401947611795984</v>
@@ -9343,6 +10811,9 @@
         <f>GETPIVOTDATA("Sum of ZEROR-residual",$A$3,"next term",6)/$F$8</f>
         <v>0.76561406026647272</v>
       </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
       <c r="M8">
         <f t="shared" si="0"/>
         <v>0.11265050681501694</v>
@@ -9396,6 +10867,9 @@
         <f>GETPIVOTDATA("Sum of ZEROR-residual",$A$3,"next term",7)/$F$9</f>
         <v>0.71470256736429838</v>
       </c>
+      <c r="L9">
+        <v>7</v>
+      </c>
       <c r="M9">
         <f t="shared" si="0"/>
         <v>6.4098153328822655E-2</v>
@@ -9449,6 +10923,9 @@
         <f>GETPIVOTDATA("Sum of ZEROR-residual",$A$3,"next term",8)/$F$10</f>
         <v>0.68000619276619201</v>
       </c>
+      <c r="L10">
+        <v>8</v>
+      </c>
       <c r="M10">
         <f t="shared" si="0"/>
         <v>6.3274726130732761E-2</v>
@@ -9502,6 +10979,9 @@
         <f>GETPIVOTDATA("Sum of ZEROR-residual",$A$3,"next term",9)/$F$11</f>
         <v>0.81665587200302625</v>
       </c>
+      <c r="L11">
+        <v>9</v>
+      </c>
       <c r="M11">
         <f t="shared" si="0"/>
         <v>0.1224465756653058</v>
@@ -9555,6 +11035,9 @@
         <f>GETPIVOTDATA("Sum of ZEROR-residual",$A$3,"next term",10)/$F$12</f>
         <v>0.37251329939594169</v>
       </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
       <c r="M12">
         <f t="shared" si="0"/>
         <v>9.0335856361957539E-2</v>
@@ -9608,6 +11091,9 @@
         <f>GETPIVOTDATA("Sum of ZEROR-residual",$A$3,"next term",11)/$F$13</f>
         <v>0.55093498155274689</v>
       </c>
+      <c r="L13">
+        <v>11</v>
+      </c>
       <c r="M13">
         <f t="shared" si="0"/>
         <v>0.20128181654328492</v>
@@ -9661,6 +11147,9 @@
         <f>GETPIVOTDATA("Sum of ZEROR-residual",$A$3,"next term",12)/$F$14</f>
         <v>0.23147980959170653</v>
       </c>
+      <c r="L14">
+        <v>12</v>
+      </c>
       <c r="M14">
         <f t="shared" si="0"/>
         <v>2.2578072171061229E-2</v>
@@ -9714,6 +11203,9 @@
         <f>GETPIVOTDATA("Sum of ZEROR-residual",$A$3,"next term",13)/$F$15</f>
         <v>0.67395147785105036</v>
       </c>
+      <c r="L15">
+        <v>13</v>
+      </c>
       <c r="M15">
         <f t="shared" si="0"/>
         <v>0.12728645909545466</v>
@@ -9767,6 +11259,9 @@
         <f>GETPIVOTDATA("Sum of ZEROR-residual",$A$3,"next term",14)/$F$16</f>
         <v>0.29859652715409801</v>
       </c>
+      <c r="L16">
+        <v>14</v>
+      </c>
       <c r="M16">
         <f t="shared" si="0"/>
         <v>0.55977077266133157</v>
@@ -9802,11 +11297,24 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U562"/>
   <sheetViews>

</xml_diff>